<commit_message>
panjin but housed value and disadvantaged values are not set yet
</commit_message>
<xml_diff>
--- a/management/客户买车行为.xlsx
+++ b/management/客户买车行为.xlsx
@@ -12,11 +12,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17610"/>
   </bookViews>
   <sheets>
-    <sheet name="A13" sheetId="5" r:id="rId1"/>
-    <sheet name="General Values" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId5"/>
+    <sheet name="Panjin" sheetId="6" r:id="rId1"/>
+    <sheet name="A13" sheetId="5" r:id="rId2"/>
+    <sheet name="General Values" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="65">
   <si>
     <t>住宅总建筑面积</t>
   </si>
@@ -217,6 +218,12 @@
   </si>
   <si>
     <t>11层小高</t>
+  </si>
+  <si>
+    <t>BaseIncomeNumber</t>
+  </si>
+  <si>
+    <t>ExponentBase</t>
   </si>
 </sst>
 </file>
@@ -441,6 +448,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -456,7 +464,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="千位分隔" xfId="2" builtinId="3"/>
@@ -742,14 +749,14 @@
   <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="12" customWidth="1"/>
-    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -757,12 +764,20 @@
         <v>18</v>
       </c>
     </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2">
+        <v>1.5</v>
+      </c>
+    </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -839,14 +854,14 @@
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
-      <c r="D11" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>61</v>
+      <c r="D11" s="13">
+        <v>125</v>
+      </c>
+      <c r="E11" s="13">
+        <v>140</v>
+      </c>
+      <c r="F11" s="13">
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -854,24 +869,24 @@
         <v>51</v>
       </c>
       <c r="B12" s="17">
-        <f>$B$3*1.5^B9</f>
-        <v>10</v>
+        <f>$B$3*$B$2^B9</f>
+        <v>8</v>
       </c>
       <c r="C12" s="17">
-        <f t="shared" ref="C12:F12" si="0">$B$3*1.5^C9</f>
-        <v>15</v>
+        <f t="shared" ref="C12:F12" si="0">$B$3*$B$2^C9</f>
+        <v>12</v>
       </c>
       <c r="D12" s="17">
         <f t="shared" si="0"/>
-        <v>22.5</v>
+        <v>18</v>
       </c>
       <c r="E12" s="17">
         <f t="shared" si="0"/>
-        <v>33.75</v>
+        <v>27</v>
       </c>
       <c r="F12" s="17">
         <f t="shared" si="0"/>
-        <v>50.625</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -879,44 +894,44 @@
         <v>30</v>
       </c>
       <c r="B13" s="19">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="C13" s="19">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="D13" s="19">
-        <v>0.35</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E13" s="19">
-        <v>0.3</v>
+        <v>0.24</v>
       </c>
       <c r="F13" s="19">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="34">
+      <c r="B14" s="29">
         <f>B12*B13</f>
-        <v>4.5</v>
-      </c>
-      <c r="C14" s="34">
+        <v>3.2</v>
+      </c>
+      <c r="C14" s="29">
         <f>C12*C13</f>
-        <v>6</v>
-      </c>
-      <c r="D14" s="34">
+        <v>4.1999999999999993</v>
+      </c>
+      <c r="D14" s="29">
         <f>D12*D13</f>
-        <v>7.8749999999999991</v>
-      </c>
-      <c r="E14" s="34">
+        <v>5.0400000000000009</v>
+      </c>
+      <c r="E14" s="29">
         <f>E12*E13</f>
-        <v>10.125</v>
-      </c>
-      <c r="F14" s="34">
+        <v>6.4799999999999995</v>
+      </c>
+      <c r="F14" s="29">
         <f>F12*F13</f>
-        <v>12.65625</v>
+        <v>8.91</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -924,44 +939,44 @@
         <v>32</v>
       </c>
       <c r="B15" s="18">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C15" s="18">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D15" s="18">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E15" s="18">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F15" s="18">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="34">
+      <c r="B16" s="29">
         <f>B15*B14</f>
-        <v>112.5</v>
-      </c>
-      <c r="C16" s="34">
+        <v>51.2</v>
+      </c>
+      <c r="C16" s="29">
         <f>C15*C14</f>
-        <v>150</v>
-      </c>
-      <c r="D16" s="34">
+        <v>67.199999999999989</v>
+      </c>
+      <c r="D16" s="29">
         <f>D15*D14</f>
-        <v>196.87499999999997</v>
-      </c>
-      <c r="E16" s="34">
+        <v>80.640000000000015</v>
+      </c>
+      <c r="E16" s="29">
         <f>E15*E14</f>
-        <v>253.125</v>
-      </c>
-      <c r="F16" s="34">
+        <v>97.199999999999989</v>
+      </c>
+      <c r="F16" s="29">
         <f>F15*F14</f>
-        <v>316.40625</v>
+        <v>124.74000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -970,23 +985,23 @@
       </c>
       <c r="B17" s="18">
         <f>B16/B12</f>
-        <v>11.25</v>
+        <v>6.4</v>
       </c>
       <c r="C17" s="18">
         <f>C16/C12</f>
-        <v>10</v>
+        <v>5.5999999999999988</v>
       </c>
       <c r="D17" s="18">
         <f>D16/D12</f>
-        <v>8.7499999999999982</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="E17" s="18">
         <f>E16/E12</f>
-        <v>7.5</v>
+        <v>3.5999999999999996</v>
       </c>
       <c r="F17" s="18">
         <f>F16/F12</f>
-        <v>6.25</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1002,19 +1017,19 @@
         <v>52</v>
       </c>
       <c r="B19" s="18">
-        <v>12000</v>
+        <v>5000</v>
       </c>
       <c r="C19" s="18">
-        <v>13000</v>
+        <v>5300</v>
       </c>
       <c r="D19" s="18">
-        <v>14000</v>
+        <v>6500</v>
       </c>
       <c r="E19" s="18">
-        <v>16500</v>
+        <v>7000</v>
       </c>
       <c r="F19" s="18">
-        <v>19000</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1023,23 +1038,23 @@
       </c>
       <c r="B20" s="20">
         <f>B16*10000/B19</f>
-        <v>93.75</v>
+        <v>102.4</v>
       </c>
       <c r="C20" s="20">
         <f t="shared" ref="C20:F20" si="1">C16*10000/C19</f>
-        <v>115.38461538461539</v>
+        <v>126.79245283018865</v>
       </c>
       <c r="D20" s="20">
         <f t="shared" si="1"/>
-        <v>140.62499999999997</v>
+        <v>124.06153846153848</v>
       </c>
       <c r="E20" s="20">
         <f t="shared" si="1"/>
-        <v>153.40909090909091</v>
+        <v>138.85714285714283</v>
       </c>
       <c r="F20" s="20">
         <f t="shared" si="1"/>
-        <v>166.52960526315789</v>
+        <v>166.32</v>
       </c>
       <c r="K20" s="12">
         <v>0.8</v>
@@ -1071,19 +1086,19 @@
         <v>45</v>
       </c>
       <c r="B22" s="19">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="C22" s="19">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="D22" s="19">
         <v>0.12</v>
       </c>
       <c r="E22" s="19">
+        <v>0.11</v>
+      </c>
+      <c r="F22" s="19">
         <v>0.1</v>
-      </c>
-      <c r="F22" s="19">
-        <v>0.09</v>
       </c>
       <c r="K22">
         <f>K20*K21</f>
@@ -1104,23 +1119,23 @@
       </c>
       <c r="B23" s="18">
         <f>B12*B22*10000</f>
-        <v>15000</v>
+        <v>8000</v>
       </c>
       <c r="C23" s="18">
         <f t="shared" ref="C23:F23" si="2">C12*C22*10000</f>
-        <v>19500</v>
+        <v>13200</v>
       </c>
       <c r="D23" s="18">
         <f t="shared" si="2"/>
-        <v>26999.999999999996</v>
+        <v>21600</v>
       </c>
       <c r="E23" s="18">
         <f t="shared" si="2"/>
-        <v>33750</v>
+        <v>29700.000000000004</v>
       </c>
       <c r="F23" s="18">
         <f t="shared" si="2"/>
-        <v>45562.499999999993</v>
+        <v>40500</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1131,16 +1146,16 @@
         <v>9000</v>
       </c>
       <c r="C24" s="18">
+        <v>9500</v>
+      </c>
+      <c r="D24" s="18">
         <v>10000</v>
       </c>
-      <c r="D24" s="18">
+      <c r="E24" s="18">
+        <v>11000</v>
+      </c>
+      <c r="F24" s="18">
         <v>12000</v>
-      </c>
-      <c r="E24" s="18">
-        <v>15000</v>
-      </c>
-      <c r="F24" s="18">
-        <v>20000</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -1149,23 +1164,23 @@
       </c>
       <c r="B25" s="18">
         <f>(B23-B24)*10</f>
-        <v>60000</v>
+        <v>-10000</v>
       </c>
       <c r="C25" s="18">
         <f t="shared" ref="C25:F25" si="3">(C23-C24)*10</f>
-        <v>95000</v>
+        <v>37000</v>
       </c>
       <c r="D25" s="18">
         <f t="shared" si="3"/>
-        <v>149999.99999999997</v>
+        <v>116000</v>
       </c>
       <c r="E25" s="18">
         <f t="shared" si="3"/>
-        <v>187500</v>
+        <v>187000.00000000003</v>
       </c>
       <c r="F25" s="18">
         <f t="shared" si="3"/>
-        <v>255624.99999999994</v>
+        <v>285000</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -1208,75 +1223,75 @@
       <c r="A29" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="34">
+      <c r="B29" s="29">
         <f>B12*10000/$B$5</f>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="C29" s="34">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C29" s="29">
         <f>C12*10000/$B$5</f>
-        <v>1.25</v>
-      </c>
-      <c r="D29" s="34">
+        <v>1</v>
+      </c>
+      <c r="D29" s="29">
         <f>D12*10000/$B$5</f>
-        <v>1.875</v>
-      </c>
-      <c r="E29" s="34">
+        <v>1.5</v>
+      </c>
+      <c r="E29" s="29">
         <f>E12*10000/$B$5</f>
-        <v>2.8125</v>
-      </c>
-      <c r="F29" s="34">
+        <v>2.25</v>
+      </c>
+      <c r="F29" s="29">
         <f>F12*10000/$B$5</f>
-        <v>4.21875</v>
+        <v>3.375</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="34">
+      <c r="B30" s="29">
         <f>B29*$B$6/80</f>
-        <v>6.25</v>
-      </c>
-      <c r="C30" s="34">
-        <f t="shared" ref="C30:F30" si="4">C29*$B$6/80</f>
-        <v>9.375</v>
-      </c>
-      <c r="D30" s="34">
+        <v>5</v>
+      </c>
+      <c r="C30" s="29">
+        <f t="shared" ref="C30:E30" si="4">C29*$B$6/80</f>
+        <v>7.5</v>
+      </c>
+      <c r="D30" s="29">
         <f t="shared" si="4"/>
-        <v>14.0625</v>
-      </c>
-      <c r="E30" s="34">
+        <v>11.25</v>
+      </c>
+      <c r="E30" s="29">
         <f t="shared" si="4"/>
-        <v>21.09375</v>
-      </c>
-      <c r="F30" s="34">
+        <v>16.875</v>
+      </c>
+      <c r="F30" s="29">
         <f>F29*$B$6/80</f>
-        <v>31.640625</v>
+        <v>25.3125</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="34">
+      <c r="B31" s="29">
         <f>B30*$B$7</f>
-        <v>156.25</v>
-      </c>
-      <c r="C31" s="34">
-        <f t="shared" ref="C31:F31" si="5">C30*$B$7</f>
-        <v>234.375</v>
-      </c>
-      <c r="D31" s="34">
+        <v>125</v>
+      </c>
+      <c r="C31" s="29">
+        <f t="shared" ref="C31:E31" si="5">C30*$B$7</f>
+        <v>187.5</v>
+      </c>
+      <c r="D31" s="29">
         <f t="shared" si="5"/>
-        <v>351.5625</v>
-      </c>
-      <c r="E31" s="34">
+        <v>281.25</v>
+      </c>
+      <c r="E31" s="29">
         <f t="shared" si="5"/>
-        <v>527.34375</v>
-      </c>
-      <c r="F31" s="34">
+        <v>421.875</v>
+      </c>
+      <c r="F31" s="29">
         <f>F30*$B$7</f>
-        <v>791.015625</v>
+        <v>632.8125</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -1328,23 +1343,23 @@
       </c>
       <c r="B35" s="23">
         <f t="shared" si="6"/>
-        <v>7812.5</v>
+        <v>6250</v>
       </c>
       <c r="C35" s="23">
         <f t="shared" si="6"/>
-        <v>11718.75</v>
+        <v>9375</v>
       </c>
       <c r="D35" s="23">
         <f t="shared" si="6"/>
-        <v>17578.125</v>
+        <v>14062.5</v>
       </c>
       <c r="E35" s="23">
         <f t="shared" si="6"/>
-        <v>26367.1875</v>
+        <v>21093.75</v>
       </c>
       <c r="F35" s="23">
         <f t="shared" si="6"/>
-        <v>39550.78125</v>
+        <v>31640.625</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1353,23 +1368,23 @@
       </c>
       <c r="B36" s="23">
         <f t="shared" si="6"/>
-        <v>15625</v>
+        <v>12500</v>
       </c>
       <c r="C36" s="23">
         <f t="shared" si="6"/>
-        <v>23437.5</v>
+        <v>18750</v>
       </c>
       <c r="D36" s="23">
         <f t="shared" si="6"/>
-        <v>35156.25</v>
+        <v>28125</v>
       </c>
       <c r="E36" s="23">
         <f t="shared" si="6"/>
-        <v>52734.375</v>
+        <v>42187.5</v>
       </c>
       <c r="F36" s="23">
         <f t="shared" si="6"/>
-        <v>79101.5625</v>
+        <v>63281.25</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1378,23 +1393,23 @@
       </c>
       <c r="B37" s="23">
         <f t="shared" si="6"/>
-        <v>23437.5</v>
+        <v>18750</v>
       </c>
       <c r="C37" s="23">
         <f t="shared" si="6"/>
-        <v>35156.25</v>
+        <v>28125</v>
       </c>
       <c r="D37" s="23">
         <f t="shared" si="6"/>
-        <v>52734.375</v>
+        <v>42187.5</v>
       </c>
       <c r="E37" s="23">
         <f t="shared" si="6"/>
-        <v>79101.5625</v>
+        <v>63281.25</v>
       </c>
       <c r="F37" s="23">
         <f t="shared" si="6"/>
-        <v>118652.34375</v>
+        <v>94921.875</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1403,23 +1418,23 @@
       </c>
       <c r="B38" s="23">
         <f t="shared" si="6"/>
-        <v>31250</v>
+        <v>25000</v>
       </c>
       <c r="C38" s="23">
         <f t="shared" si="6"/>
-        <v>46875</v>
+        <v>37500</v>
       </c>
       <c r="D38" s="23">
         <f t="shared" si="6"/>
-        <v>70312.5</v>
+        <v>56250</v>
       </c>
       <c r="E38" s="23">
         <f t="shared" si="6"/>
-        <v>105468.75</v>
+        <v>84375</v>
       </c>
       <c r="F38" s="23">
         <f t="shared" si="6"/>
-        <v>158203.125</v>
+        <v>126562.5</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1428,23 +1443,23 @@
       </c>
       <c r="B39" s="23">
         <f t="shared" si="6"/>
-        <v>39062.5</v>
+        <v>31250</v>
       </c>
       <c r="C39" s="23">
         <f t="shared" si="6"/>
-        <v>58593.75</v>
+        <v>46875</v>
       </c>
       <c r="D39" s="23">
         <f t="shared" si="6"/>
-        <v>87890.625</v>
+        <v>70312.5</v>
       </c>
       <c r="E39" s="23">
         <f t="shared" si="6"/>
-        <v>131835.9375</v>
+        <v>105468.75</v>
       </c>
       <c r="F39" s="23">
         <f t="shared" si="6"/>
-        <v>197753.90625</v>
+        <v>158203.125</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1453,23 +1468,23 @@
       </c>
       <c r="B40" s="23">
         <f t="shared" si="6"/>
-        <v>46875</v>
+        <v>37500</v>
       </c>
       <c r="C40" s="23">
         <f t="shared" si="6"/>
-        <v>70312.5</v>
+        <v>56250</v>
       </c>
       <c r="D40" s="23">
         <f t="shared" si="6"/>
-        <v>105468.75</v>
+        <v>84375</v>
       </c>
       <c r="E40" s="23">
         <f t="shared" si="6"/>
-        <v>158203.125</v>
+        <v>126562.5</v>
       </c>
       <c r="F40" s="23">
         <f t="shared" si="6"/>
-        <v>237304.6875</v>
+        <v>189843.75</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1478,23 +1493,23 @@
       </c>
       <c r="B41" s="23">
         <f t="shared" si="6"/>
-        <v>54687.5</v>
+        <v>43750</v>
       </c>
       <c r="C41" s="23">
         <f t="shared" si="6"/>
-        <v>82031.25</v>
+        <v>65625</v>
       </c>
       <c r="D41" s="23">
         <f t="shared" si="6"/>
-        <v>123046.875</v>
+        <v>98437.5</v>
       </c>
       <c r="E41" s="23">
         <f t="shared" si="6"/>
-        <v>184570.3125</v>
+        <v>147656.25</v>
       </c>
       <c r="F41" s="23">
         <f t="shared" si="6"/>
-        <v>276855.46875</v>
+        <v>221484.375</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1503,23 +1518,23 @@
       </c>
       <c r="B42" s="23">
         <f t="shared" si="6"/>
-        <v>62500</v>
+        <v>50000</v>
       </c>
       <c r="C42" s="23">
         <f t="shared" si="6"/>
-        <v>93750</v>
+        <v>75000</v>
       </c>
       <c r="D42" s="23">
         <f t="shared" si="6"/>
-        <v>140625</v>
+        <v>112500</v>
       </c>
       <c r="E42" s="23">
         <f t="shared" si="6"/>
-        <v>210937.5</v>
+        <v>168750</v>
       </c>
       <c r="F42" s="23">
         <f t="shared" si="6"/>
-        <v>316406.25</v>
+        <v>253125</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1538,23 +1553,23 @@
       </c>
       <c r="B44" s="23">
         <f>B42</f>
-        <v>62500</v>
+        <v>50000</v>
       </c>
       <c r="C44" s="25">
         <f t="shared" ref="C44:F44" si="7">C42</f>
-        <v>93750</v>
+        <v>75000</v>
       </c>
       <c r="D44" s="25">
         <f t="shared" si="7"/>
-        <v>140625</v>
+        <v>112500</v>
       </c>
       <c r="E44" s="25">
         <f t="shared" si="7"/>
-        <v>210937.5</v>
+        <v>168750</v>
       </c>
       <c r="F44" s="23">
         <f t="shared" si="7"/>
-        <v>316406.25</v>
+        <v>253125</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1563,23 +1578,23 @@
       </c>
       <c r="B45" s="23">
         <f>B$44-B35</f>
-        <v>54687.5</v>
+        <v>43750</v>
       </c>
       <c r="C45" s="25">
         <f t="shared" ref="C45:F45" si="8">C$44-C35</f>
-        <v>82031.25</v>
+        <v>65625</v>
       </c>
       <c r="D45" s="25">
         <f t="shared" si="8"/>
-        <v>123046.875</v>
+        <v>98437.5</v>
       </c>
       <c r="E45" s="25">
         <f t="shared" si="8"/>
-        <v>184570.3125</v>
+        <v>147656.25</v>
       </c>
       <c r="F45" s="23">
         <f t="shared" si="8"/>
-        <v>276855.46875</v>
+        <v>221484.375</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1588,23 +1603,23 @@
       </c>
       <c r="B46" s="23">
         <f t="shared" ref="B46:F52" si="9">B$44-B36</f>
-        <v>46875</v>
+        <v>37500</v>
       </c>
       <c r="C46" s="25">
         <f t="shared" si="9"/>
-        <v>70312.5</v>
+        <v>56250</v>
       </c>
       <c r="D46" s="25">
         <f t="shared" si="9"/>
-        <v>105468.75</v>
+        <v>84375</v>
       </c>
       <c r="E46" s="25">
         <f t="shared" si="9"/>
-        <v>158203.125</v>
+        <v>126562.5</v>
       </c>
       <c r="F46" s="23">
         <f t="shared" si="9"/>
-        <v>237304.6875</v>
+        <v>189843.75</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1613,23 +1628,23 @@
       </c>
       <c r="B47" s="23">
         <f t="shared" si="9"/>
-        <v>39062.5</v>
+        <v>31250</v>
       </c>
       <c r="C47" s="23">
         <f t="shared" si="9"/>
-        <v>58593.75</v>
+        <v>46875</v>
       </c>
       <c r="D47" s="23">
         <f t="shared" si="9"/>
-        <v>87890.625</v>
+        <v>70312.5</v>
       </c>
       <c r="E47" s="23">
         <f t="shared" si="9"/>
-        <v>131835.9375</v>
+        <v>105468.75</v>
       </c>
       <c r="F47" s="23">
         <f t="shared" si="9"/>
-        <v>197753.90625</v>
+        <v>158203.125</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1638,23 +1653,23 @@
       </c>
       <c r="B48" s="23">
         <f t="shared" si="9"/>
-        <v>31250</v>
+        <v>25000</v>
       </c>
       <c r="C48" s="23">
         <f t="shared" si="9"/>
-        <v>46875</v>
+        <v>37500</v>
       </c>
       <c r="D48" s="23">
         <f t="shared" si="9"/>
-        <v>70312.5</v>
+        <v>56250</v>
       </c>
       <c r="E48" s="23">
         <f t="shared" si="9"/>
-        <v>105468.75</v>
+        <v>84375</v>
       </c>
       <c r="F48" s="23">
         <f t="shared" si="9"/>
-        <v>158203.125</v>
+        <v>126562.5</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1663,23 +1678,23 @@
       </c>
       <c r="B49" s="23">
         <f t="shared" si="9"/>
-        <v>23437.5</v>
+        <v>18750</v>
       </c>
       <c r="C49" s="23">
         <f t="shared" si="9"/>
-        <v>35156.25</v>
+        <v>28125</v>
       </c>
       <c r="D49" s="23">
         <f t="shared" si="9"/>
-        <v>52734.375</v>
+        <v>42187.5</v>
       </c>
       <c r="E49" s="23">
         <f t="shared" si="9"/>
-        <v>79101.5625</v>
+        <v>63281.25</v>
       </c>
       <c r="F49" s="23">
         <f t="shared" si="9"/>
-        <v>118652.34375</v>
+        <v>94921.875</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1688,23 +1703,23 @@
       </c>
       <c r="B50" s="23">
         <f t="shared" si="9"/>
-        <v>15625</v>
+        <v>12500</v>
       </c>
       <c r="C50" s="23">
         <f t="shared" si="9"/>
-        <v>23437.5</v>
+        <v>18750</v>
       </c>
       <c r="D50" s="23">
         <f t="shared" si="9"/>
-        <v>35156.25</v>
+        <v>28125</v>
       </c>
       <c r="E50" s="23">
         <f t="shared" si="9"/>
-        <v>52734.375</v>
+        <v>42187.5</v>
       </c>
       <c r="F50" s="23">
         <f t="shared" si="9"/>
-        <v>79101.5625</v>
+        <v>63281.25</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1713,23 +1728,23 @@
       </c>
       <c r="B51" s="23">
         <f t="shared" si="9"/>
-        <v>7812.5</v>
+        <v>6250</v>
       </c>
       <c r="C51" s="23">
         <f t="shared" si="9"/>
-        <v>11718.75</v>
+        <v>9375</v>
       </c>
       <c r="D51" s="23">
         <f t="shared" si="9"/>
-        <v>17578.125</v>
+        <v>14062.5</v>
       </c>
       <c r="E51" s="23">
         <f t="shared" si="9"/>
-        <v>26367.1875</v>
+        <v>21093.75</v>
       </c>
       <c r="F51" s="23">
         <f t="shared" si="9"/>
-        <v>39550.78125</v>
+        <v>31640.625</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1817,23 +1832,23 @@
       </c>
       <c r="B58" s="27">
         <f>B57/B12/10000</f>
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="C58" s="27">
         <f t="shared" ref="C58:F58" si="11">C57/C12/10000</f>
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="D58" s="27">
         <f t="shared" si="11"/>
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="E58" s="27">
         <f t="shared" si="11"/>
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="F58" s="27">
         <f t="shared" si="11"/>
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -1862,23 +1877,23 @@
       </c>
       <c r="B60" s="12">
         <f>B59-B58</f>
-        <v>0</v>
+        <v>-0.03</v>
       </c>
       <c r="C60" s="12">
         <f t="shared" ref="C60:F60" si="12">C59-C58</f>
-        <v>0</v>
+        <v>-0.03</v>
       </c>
       <c r="D60" s="12">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-0.03</v>
       </c>
       <c r="E60" s="12">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-0.03</v>
       </c>
       <c r="F60" s="12">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -1887,23 +1902,23 @@
       </c>
       <c r="B61" s="12">
         <f>B59/B58</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C61" s="12">
         <f t="shared" ref="C61:F61" si="13">C59/C58</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D61" s="12">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E61" s="12">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F61" s="12">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -1917,14 +1932,14 @@
   <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="12" customWidth="1"/>
-    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1937,7 +1952,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2012,20 +2027,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="13"/>
-      <c r="B11" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>41</v>
-      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="13" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2033,24 +2044,24 @@
         <v>51</v>
       </c>
       <c r="B12" s="17">
-        <f>$B$3*2^B9</f>
-        <v>6</v>
+        <f>$B$3*1.5^B9</f>
+        <v>10</v>
       </c>
       <c r="C12" s="17">
-        <f>$B$3*2^C9</f>
-        <v>12</v>
+        <f t="shared" ref="C12:F12" si="0">$B$3*1.5^C9</f>
+        <v>15</v>
       </c>
       <c r="D12" s="17">
-        <f>$B$3*2^D9</f>
-        <v>24</v>
+        <f t="shared" si="0"/>
+        <v>22.5</v>
       </c>
       <c r="E12" s="17">
-        <f>$B$3*2^E9</f>
-        <v>48</v>
+        <f t="shared" si="0"/>
+        <v>33.75</v>
       </c>
       <c r="F12" s="17">
-        <f>$B$3*2^F9</f>
-        <v>96</v>
+        <f t="shared" si="0"/>
+        <v>50.625</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2058,44 +2069,44 @@
         <v>30</v>
       </c>
       <c r="B13" s="19">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="C13" s="19">
         <v>0.4</v>
       </c>
       <c r="D13" s="19">
-        <v>0.28000000000000003</v>
+        <v>0.35</v>
       </c>
       <c r="E13" s="19">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F13" s="19">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="29">
         <f>B12*B13</f>
-        <v>3</v>
-      </c>
-      <c r="C14" s="18">
+        <v>4.5</v>
+      </c>
+      <c r="C14" s="29">
         <f>C12*C13</f>
-        <v>4.8000000000000007</v>
-      </c>
-      <c r="D14" s="18">
+        <v>6</v>
+      </c>
+      <c r="D14" s="29">
         <f>D12*D13</f>
-        <v>6.7200000000000006</v>
-      </c>
-      <c r="E14" s="18">
+        <v>7.8749999999999991</v>
+      </c>
+      <c r="E14" s="29">
         <f>E12*E13</f>
-        <v>9.6000000000000014</v>
-      </c>
-      <c r="F14" s="18">
+        <v>10.125</v>
+      </c>
+      <c r="F14" s="29">
         <f>F12*F13</f>
-        <v>14.399999999999999</v>
+        <v>12.65625</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2122,25 +2133,25 @@
       <c r="A16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="29">
         <f>B15*B14</f>
-        <v>75</v>
-      </c>
-      <c r="C16" s="18">
+        <v>112.5</v>
+      </c>
+      <c r="C16" s="29">
         <f>C15*C14</f>
-        <v>120.00000000000001</v>
-      </c>
-      <c r="D16" s="18">
+        <v>150</v>
+      </c>
+      <c r="D16" s="29">
         <f>D15*D14</f>
-        <v>168.00000000000003</v>
-      </c>
-      <c r="E16" s="18">
+        <v>196.87499999999997</v>
+      </c>
+      <c r="E16" s="29">
         <f>E15*E14</f>
-        <v>240.00000000000003</v>
-      </c>
-      <c r="F16" s="18">
+        <v>253.125</v>
+      </c>
+      <c r="F16" s="29">
         <f>F15*F14</f>
-        <v>359.99999999999994</v>
+        <v>316.40625</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -2149,23 +2160,23 @@
       </c>
       <c r="B17" s="18">
         <f>B16/B12</f>
-        <v>12.5</v>
+        <v>11.25</v>
       </c>
       <c r="C17" s="18">
         <f>C16/C12</f>
-        <v>10.000000000000002</v>
+        <v>10</v>
       </c>
       <c r="D17" s="18">
         <f>D16/D12</f>
-        <v>7.0000000000000009</v>
+        <v>8.7499999999999982</v>
       </c>
       <c r="E17" s="18">
         <f>E16/E12</f>
-        <v>5.0000000000000009</v>
+        <v>7.5</v>
       </c>
       <c r="F17" s="18">
         <f>F16/F12</f>
-        <v>3.7499999999999996</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -2181,19 +2192,19 @@
         <v>52</v>
       </c>
       <c r="B19" s="18">
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="C19" s="18">
-        <v>12000</v>
+        <v>13000</v>
       </c>
       <c r="D19" s="18">
         <v>14000</v>
       </c>
       <c r="E19" s="18">
-        <v>16000</v>
+        <v>16500</v>
       </c>
       <c r="F19" s="18">
-        <v>18000</v>
+        <v>19000</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -2202,23 +2213,23 @@
       </c>
       <c r="B20" s="20">
         <f>B16*10000/B19</f>
-        <v>83.333333333333329</v>
+        <v>93.75</v>
       </c>
       <c r="C20" s="20">
-        <f t="shared" ref="C20:F20" si="0">C16*10000/C19</f>
-        <v>100.00000000000001</v>
+        <f t="shared" ref="C20:F20" si="1">C16*10000/C19</f>
+        <v>115.38461538461539</v>
       </c>
       <c r="D20" s="20">
-        <f t="shared" si="0"/>
-        <v>120.00000000000001</v>
+        <f t="shared" si="1"/>
+        <v>140.62499999999997</v>
       </c>
       <c r="E20" s="20">
-        <f t="shared" si="0"/>
-        <v>150.00000000000003</v>
+        <f t="shared" si="1"/>
+        <v>153.40909090909091</v>
       </c>
       <c r="F20" s="20">
-        <f t="shared" si="0"/>
-        <v>199.99999999999997</v>
+        <f t="shared" si="1"/>
+        <v>166.52960526315789</v>
       </c>
       <c r="K20" s="12">
         <v>0.8</v>
@@ -2283,23 +2294,23 @@
       </c>
       <c r="B23" s="18">
         <f>B12*B22*10000</f>
-        <v>9000</v>
+        <v>15000</v>
       </c>
       <c r="C23" s="18">
-        <f t="shared" ref="C23:F23" si="1">C12*C22*10000</f>
-        <v>15600</v>
+        <f t="shared" ref="C23:F23" si="2">C12*C22*10000</f>
+        <v>19500</v>
       </c>
       <c r="D23" s="18">
-        <f t="shared" si="1"/>
-        <v>28800</v>
+        <f t="shared" si="2"/>
+        <v>26999.999999999996</v>
       </c>
       <c r="E23" s="18">
-        <f t="shared" si="1"/>
-        <v>48000.000000000007</v>
+        <f t="shared" si="2"/>
+        <v>33750</v>
       </c>
       <c r="F23" s="18">
-        <f t="shared" si="1"/>
-        <v>86400</v>
+        <f t="shared" si="2"/>
+        <v>45562.499999999993</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -2328,23 +2339,23 @@
       </c>
       <c r="B25" s="18">
         <f>(B23-B24)*10</f>
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="C25" s="18">
-        <f t="shared" ref="C25:F25" si="2">(C23-C24)*10</f>
-        <v>56000</v>
+        <f t="shared" ref="C25:F25" si="3">(C23-C24)*10</f>
+        <v>95000</v>
       </c>
       <c r="D25" s="18">
-        <f t="shared" si="2"/>
-        <v>168000</v>
+        <f t="shared" si="3"/>
+        <v>149999.99999999997</v>
       </c>
       <c r="E25" s="18">
-        <f t="shared" si="2"/>
-        <v>330000.00000000006</v>
+        <f t="shared" si="3"/>
+        <v>187500</v>
       </c>
       <c r="F25" s="18">
-        <f t="shared" si="2"/>
-        <v>664000</v>
+        <f t="shared" si="3"/>
+        <v>255624.99999999994</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -2387,75 +2398,75 @@
       <c r="A29" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="29">
         <f>B12*10000/$B$5</f>
-        <v>0.5</v>
-      </c>
-      <c r="C29" s="18">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C29" s="29">
         <f>C12*10000/$B$5</f>
-        <v>1</v>
-      </c>
-      <c r="D29" s="18">
+        <v>1.25</v>
+      </c>
+      <c r="D29" s="29">
         <f>D12*10000/$B$5</f>
-        <v>2</v>
-      </c>
-      <c r="E29" s="18">
+        <v>1.875</v>
+      </c>
+      <c r="E29" s="29">
         <f>E12*10000/$B$5</f>
-        <v>4</v>
-      </c>
-      <c r="F29" s="18">
+        <v>2.8125</v>
+      </c>
+      <c r="F29" s="29">
         <f>F12*10000/$B$5</f>
-        <v>8</v>
+        <v>4.21875</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="29">
         <f>B29*$B$6/80</f>
-        <v>3.75</v>
-      </c>
-      <c r="C30" s="18">
-        <f t="shared" ref="C30:F30" si="3">C29*$B$6/80</f>
-        <v>7.5</v>
-      </c>
-      <c r="D30" s="18">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="E30" s="18">
-        <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="F30" s="18">
-        <f t="shared" si="3"/>
-        <v>60</v>
+        <v>6.25</v>
+      </c>
+      <c r="C30" s="29">
+        <f t="shared" ref="C30:E30" si="4">C29*$B$6/80</f>
+        <v>9.375</v>
+      </c>
+      <c r="D30" s="29">
+        <f t="shared" si="4"/>
+        <v>14.0625</v>
+      </c>
+      <c r="E30" s="29">
+        <f t="shared" si="4"/>
+        <v>21.09375</v>
+      </c>
+      <c r="F30" s="29">
+        <f>F29*$B$6/80</f>
+        <v>31.640625</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="18">
+      <c r="B31" s="29">
         <f>B30*$B$7</f>
-        <v>93.75</v>
-      </c>
-      <c r="C31" s="18">
-        <f t="shared" ref="C31:F31" si="4">C30*$B$7</f>
-        <v>187.5</v>
-      </c>
-      <c r="D31" s="18">
-        <f t="shared" si="4"/>
-        <v>375</v>
-      </c>
-      <c r="E31" s="18">
-        <f t="shared" si="4"/>
-        <v>750</v>
-      </c>
-      <c r="F31" s="18">
-        <f t="shared" si="4"/>
-        <v>1500</v>
+        <v>156.25</v>
+      </c>
+      <c r="C31" s="29">
+        <f t="shared" ref="C31:E31" si="5">C30*$B$7</f>
+        <v>234.375</v>
+      </c>
+      <c r="D31" s="29">
+        <f t="shared" si="5"/>
+        <v>351.5625</v>
+      </c>
+      <c r="E31" s="29">
+        <f t="shared" si="5"/>
+        <v>527.34375</v>
+      </c>
+      <c r="F31" s="29">
+        <f>F30*$B$7</f>
+        <v>791.015625</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -2481,23 +2492,23 @@
         <v>0</v>
       </c>
       <c r="B34" s="18">
-        <f t="shared" ref="B34:F42" si="5">B$31*$A34</f>
+        <f t="shared" ref="B34:F42" si="6">B$31*$A34</f>
         <v>0</v>
       </c>
       <c r="C34" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D34" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E34" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F34" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2506,24 +2517,24 @@
         <v>50</v>
       </c>
       <c r="B35" s="23">
-        <f t="shared" si="5"/>
-        <v>4687.5</v>
+        <f t="shared" si="6"/>
+        <v>7812.5</v>
       </c>
       <c r="C35" s="23">
-        <f t="shared" si="5"/>
-        <v>9375</v>
+        <f t="shared" si="6"/>
+        <v>11718.75</v>
       </c>
       <c r="D35" s="23">
-        <f t="shared" si="5"/>
-        <v>18750</v>
+        <f t="shared" si="6"/>
+        <v>17578.125</v>
       </c>
       <c r="E35" s="23">
-        <f t="shared" si="5"/>
-        <v>37500</v>
+        <f t="shared" si="6"/>
+        <v>26367.1875</v>
       </c>
       <c r="F35" s="23">
-        <f t="shared" si="5"/>
-        <v>75000</v>
+        <f t="shared" si="6"/>
+        <v>39550.78125</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2531,24 +2542,24 @@
         <v>100</v>
       </c>
       <c r="B36" s="23">
-        <f t="shared" si="5"/>
-        <v>9375</v>
+        <f t="shared" si="6"/>
+        <v>15625</v>
       </c>
       <c r="C36" s="23">
-        <f t="shared" si="5"/>
-        <v>18750</v>
+        <f t="shared" si="6"/>
+        <v>23437.5</v>
       </c>
       <c r="D36" s="23">
-        <f t="shared" si="5"/>
-        <v>37500</v>
+        <f t="shared" si="6"/>
+        <v>35156.25</v>
       </c>
       <c r="E36" s="23">
-        <f t="shared" si="5"/>
-        <v>75000</v>
+        <f t="shared" si="6"/>
+        <v>52734.375</v>
       </c>
       <c r="F36" s="23">
-        <f t="shared" si="5"/>
-        <v>150000</v>
+        <f t="shared" si="6"/>
+        <v>79101.5625</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2556,24 +2567,24 @@
         <v>150</v>
       </c>
       <c r="B37" s="23">
-        <f t="shared" si="5"/>
-        <v>14062.5</v>
+        <f t="shared" si="6"/>
+        <v>23437.5</v>
       </c>
       <c r="C37" s="23">
-        <f t="shared" si="5"/>
-        <v>28125</v>
+        <f t="shared" si="6"/>
+        <v>35156.25</v>
       </c>
       <c r="D37" s="23">
-        <f t="shared" si="5"/>
-        <v>56250</v>
+        <f t="shared" si="6"/>
+        <v>52734.375</v>
       </c>
       <c r="E37" s="23">
-        <f t="shared" si="5"/>
-        <v>112500</v>
+        <f t="shared" si="6"/>
+        <v>79101.5625</v>
       </c>
       <c r="F37" s="23">
-        <f t="shared" si="5"/>
-        <v>225000</v>
+        <f t="shared" si="6"/>
+        <v>118652.34375</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2581,24 +2592,24 @@
         <v>200</v>
       </c>
       <c r="B38" s="23">
-        <f t="shared" si="5"/>
-        <v>18750</v>
+        <f t="shared" si="6"/>
+        <v>31250</v>
       </c>
       <c r="C38" s="23">
-        <f t="shared" si="5"/>
-        <v>37500</v>
+        <f t="shared" si="6"/>
+        <v>46875</v>
       </c>
       <c r="D38" s="23">
-        <f t="shared" si="5"/>
-        <v>75000</v>
+        <f t="shared" si="6"/>
+        <v>70312.5</v>
       </c>
       <c r="E38" s="23">
-        <f t="shared" si="5"/>
-        <v>150000</v>
+        <f t="shared" si="6"/>
+        <v>105468.75</v>
       </c>
       <c r="F38" s="23">
-        <f t="shared" si="5"/>
-        <v>300000</v>
+        <f t="shared" si="6"/>
+        <v>158203.125</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2606,24 +2617,24 @@
         <v>250</v>
       </c>
       <c r="B39" s="23">
-        <f t="shared" si="5"/>
-        <v>23437.5</v>
+        <f t="shared" si="6"/>
+        <v>39062.5</v>
       </c>
       <c r="C39" s="23">
-        <f t="shared" si="5"/>
-        <v>46875</v>
+        <f t="shared" si="6"/>
+        <v>58593.75</v>
       </c>
       <c r="D39" s="23">
-        <f t="shared" si="5"/>
-        <v>93750</v>
+        <f t="shared" si="6"/>
+        <v>87890.625</v>
       </c>
       <c r="E39" s="23">
-        <f t="shared" si="5"/>
-        <v>187500</v>
+        <f t="shared" si="6"/>
+        <v>131835.9375</v>
       </c>
       <c r="F39" s="23">
-        <f t="shared" si="5"/>
-        <v>375000</v>
+        <f t="shared" si="6"/>
+        <v>197753.90625</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2631,24 +2642,24 @@
         <v>300</v>
       </c>
       <c r="B40" s="23">
-        <f t="shared" si="5"/>
-        <v>28125</v>
+        <f t="shared" si="6"/>
+        <v>46875</v>
       </c>
       <c r="C40" s="23">
-        <f t="shared" si="5"/>
-        <v>56250</v>
+        <f t="shared" si="6"/>
+        <v>70312.5</v>
       </c>
       <c r="D40" s="23">
-        <f t="shared" si="5"/>
-        <v>112500</v>
+        <f t="shared" si="6"/>
+        <v>105468.75</v>
       </c>
       <c r="E40" s="23">
-        <f t="shared" si="5"/>
-        <v>225000</v>
+        <f t="shared" si="6"/>
+        <v>158203.125</v>
       </c>
       <c r="F40" s="23">
-        <f t="shared" si="5"/>
-        <v>450000</v>
+        <f t="shared" si="6"/>
+        <v>237304.6875</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2656,24 +2667,24 @@
         <v>350</v>
       </c>
       <c r="B41" s="23">
-        <f t="shared" si="5"/>
-        <v>32812.5</v>
+        <f t="shared" si="6"/>
+        <v>54687.5</v>
       </c>
       <c r="C41" s="23">
-        <f t="shared" si="5"/>
-        <v>65625</v>
+        <f t="shared" si="6"/>
+        <v>82031.25</v>
       </c>
       <c r="D41" s="23">
-        <f t="shared" si="5"/>
-        <v>131250</v>
+        <f t="shared" si="6"/>
+        <v>123046.875</v>
       </c>
       <c r="E41" s="23">
-        <f t="shared" si="5"/>
-        <v>262500</v>
+        <f t="shared" si="6"/>
+        <v>184570.3125</v>
       </c>
       <c r="F41" s="23">
-        <f t="shared" si="5"/>
-        <v>525000</v>
+        <f t="shared" si="6"/>
+        <v>276855.46875</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2681,24 +2692,24 @@
         <v>400</v>
       </c>
       <c r="B42" s="23">
-        <f t="shared" si="5"/>
-        <v>37500</v>
+        <f t="shared" si="6"/>
+        <v>62500</v>
       </c>
       <c r="C42" s="23">
-        <f t="shared" si="5"/>
-        <v>75000</v>
+        <f t="shared" si="6"/>
+        <v>93750</v>
       </c>
       <c r="D42" s="23">
-        <f t="shared" si="5"/>
-        <v>150000</v>
+        <f t="shared" si="6"/>
+        <v>140625</v>
       </c>
       <c r="E42" s="23">
-        <f t="shared" si="5"/>
-        <v>300000</v>
+        <f t="shared" si="6"/>
+        <v>210937.5</v>
       </c>
       <c r="F42" s="23">
-        <f t="shared" si="5"/>
-        <v>600000</v>
+        <f t="shared" si="6"/>
+        <v>316406.25</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2717,23 +2728,23 @@
       </c>
       <c r="B44" s="23">
         <f>B42</f>
-        <v>37500</v>
+        <v>62500</v>
       </c>
       <c r="C44" s="25">
-        <f t="shared" ref="C44:F44" si="6">C42</f>
-        <v>75000</v>
+        <f t="shared" ref="C44:F44" si="7">C42</f>
+        <v>93750</v>
       </c>
       <c r="D44" s="25">
-        <f t="shared" si="6"/>
-        <v>150000</v>
+        <f t="shared" si="7"/>
+        <v>140625</v>
       </c>
       <c r="E44" s="25">
-        <f t="shared" si="6"/>
-        <v>300000</v>
+        <f t="shared" si="7"/>
+        <v>210937.5</v>
       </c>
       <c r="F44" s="23">
-        <f t="shared" si="6"/>
-        <v>600000</v>
+        <f t="shared" si="7"/>
+        <v>316406.25</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2742,23 +2753,23 @@
       </c>
       <c r="B45" s="23">
         <f>B$44-B35</f>
-        <v>32812.5</v>
+        <v>54687.5</v>
       </c>
       <c r="C45" s="25">
-        <f t="shared" ref="C45:F45" si="7">C$44-C35</f>
-        <v>65625</v>
+        <f t="shared" ref="C45:F45" si="8">C$44-C35</f>
+        <v>82031.25</v>
       </c>
       <c r="D45" s="25">
-        <f t="shared" si="7"/>
-        <v>131250</v>
+        <f t="shared" si="8"/>
+        <v>123046.875</v>
       </c>
       <c r="E45" s="25">
-        <f t="shared" si="7"/>
-        <v>262500</v>
+        <f t="shared" si="8"/>
+        <v>184570.3125</v>
       </c>
       <c r="F45" s="23">
-        <f t="shared" si="7"/>
-        <v>525000</v>
+        <f t="shared" si="8"/>
+        <v>276855.46875</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2766,24 +2777,24 @@
         <v>100</v>
       </c>
       <c r="B46" s="23">
-        <f t="shared" ref="B46:F46" si="8">B$44-B36</f>
-        <v>28125</v>
+        <f t="shared" ref="B46:F52" si="9">B$44-B36</f>
+        <v>46875</v>
       </c>
       <c r="C46" s="25">
-        <f t="shared" si="8"/>
-        <v>56250</v>
+        <f t="shared" si="9"/>
+        <v>70312.5</v>
       </c>
       <c r="D46" s="25">
-        <f t="shared" si="8"/>
-        <v>112500</v>
+        <f t="shared" si="9"/>
+        <v>105468.75</v>
       </c>
       <c r="E46" s="25">
-        <f t="shared" si="8"/>
-        <v>225000</v>
+        <f t="shared" si="9"/>
+        <v>158203.125</v>
       </c>
       <c r="F46" s="23">
-        <f t="shared" si="8"/>
-        <v>450000</v>
+        <f t="shared" si="9"/>
+        <v>237304.6875</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2791,24 +2802,24 @@
         <v>150</v>
       </c>
       <c r="B47" s="23">
-        <f t="shared" ref="B47:F47" si="9">B$44-B37</f>
-        <v>23437.5</v>
+        <f t="shared" si="9"/>
+        <v>39062.5</v>
       </c>
       <c r="C47" s="23">
         <f t="shared" si="9"/>
-        <v>46875</v>
+        <v>58593.75</v>
       </c>
       <c r="D47" s="23">
         <f t="shared" si="9"/>
-        <v>93750</v>
+        <v>87890.625</v>
       </c>
       <c r="E47" s="23">
         <f t="shared" si="9"/>
-        <v>187500</v>
+        <v>131835.9375</v>
       </c>
       <c r="F47" s="23">
         <f t="shared" si="9"/>
-        <v>375000</v>
+        <v>197753.90625</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2816,24 +2827,24 @@
         <v>200</v>
       </c>
       <c r="B48" s="23">
-        <f t="shared" ref="B48:F48" si="10">B$44-B38</f>
-        <v>18750</v>
+        <f t="shared" si="9"/>
+        <v>31250</v>
       </c>
       <c r="C48" s="23">
-        <f t="shared" si="10"/>
-        <v>37500</v>
+        <f t="shared" si="9"/>
+        <v>46875</v>
       </c>
       <c r="D48" s="23">
-        <f t="shared" si="10"/>
-        <v>75000</v>
+        <f t="shared" si="9"/>
+        <v>70312.5</v>
       </c>
       <c r="E48" s="23">
-        <f t="shared" si="10"/>
-        <v>150000</v>
+        <f t="shared" si="9"/>
+        <v>105468.75</v>
       </c>
       <c r="F48" s="23">
-        <f t="shared" si="10"/>
-        <v>300000</v>
+        <f t="shared" si="9"/>
+        <v>158203.125</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2841,24 +2852,24 @@
         <v>250</v>
       </c>
       <c r="B49" s="23">
-        <f t="shared" ref="B49:F49" si="11">B$44-B39</f>
-        <v>14062.5</v>
+        <f t="shared" si="9"/>
+        <v>23437.5</v>
       </c>
       <c r="C49" s="23">
-        <f t="shared" si="11"/>
-        <v>28125</v>
+        <f t="shared" si="9"/>
+        <v>35156.25</v>
       </c>
       <c r="D49" s="23">
-        <f t="shared" si="11"/>
-        <v>56250</v>
+        <f t="shared" si="9"/>
+        <v>52734.375</v>
       </c>
       <c r="E49" s="23">
-        <f t="shared" si="11"/>
-        <v>112500</v>
+        <f t="shared" si="9"/>
+        <v>79101.5625</v>
       </c>
       <c r="F49" s="23">
-        <f t="shared" si="11"/>
-        <v>225000</v>
+        <f t="shared" si="9"/>
+        <v>118652.34375</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2866,24 +2877,24 @@
         <v>300</v>
       </c>
       <c r="B50" s="23">
-        <f t="shared" ref="B50:F50" si="12">B$44-B40</f>
-        <v>9375</v>
+        <f t="shared" si="9"/>
+        <v>15625</v>
       </c>
       <c r="C50" s="23">
-        <f t="shared" si="12"/>
-        <v>18750</v>
+        <f t="shared" si="9"/>
+        <v>23437.5</v>
       </c>
       <c r="D50" s="23">
-        <f t="shared" si="12"/>
-        <v>37500</v>
+        <f t="shared" si="9"/>
+        <v>35156.25</v>
       </c>
       <c r="E50" s="23">
-        <f t="shared" si="12"/>
-        <v>75000</v>
+        <f t="shared" si="9"/>
+        <v>52734.375</v>
       </c>
       <c r="F50" s="23">
-        <f t="shared" si="12"/>
-        <v>150000</v>
+        <f t="shared" si="9"/>
+        <v>79101.5625</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2891,24 +2902,24 @@
         <v>350</v>
       </c>
       <c r="B51" s="23">
-        <f t="shared" ref="B51:F51" si="13">B$44-B41</f>
-        <v>4687.5</v>
+        <f t="shared" si="9"/>
+        <v>7812.5</v>
       </c>
       <c r="C51" s="23">
-        <f t="shared" si="13"/>
-        <v>9375</v>
+        <f t="shared" si="9"/>
+        <v>11718.75</v>
       </c>
       <c r="D51" s="23">
-        <f t="shared" si="13"/>
-        <v>18750</v>
+        <f t="shared" si="9"/>
+        <v>17578.125</v>
       </c>
       <c r="E51" s="23">
-        <f t="shared" si="13"/>
-        <v>37500</v>
+        <f t="shared" si="9"/>
+        <v>26367.1875</v>
       </c>
       <c r="F51" s="23">
-        <f t="shared" si="13"/>
-        <v>75000</v>
+        <f t="shared" si="9"/>
+        <v>39550.78125</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2916,23 +2927,23 @@
         <v>400</v>
       </c>
       <c r="B52" s="23">
-        <f t="shared" ref="B52:F52" si="14">B$44-B42</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C52" s="23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="D52" s="23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E52" s="23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F52" s="23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2974,19 +2985,19 @@
         <v>12000</v>
       </c>
       <c r="C57" s="26">
-        <f t="shared" ref="C57:F57" si="15">$I$55*$I$56^C9</f>
+        <f t="shared" ref="C57:F57" si="10">$I$55*$I$56^C9</f>
         <v>18000</v>
       </c>
       <c r="D57" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>27000</v>
       </c>
       <c r="E57" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>40500</v>
       </c>
       <c r="F57" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>60750</v>
       </c>
     </row>
@@ -2996,23 +3007,23 @@
       </c>
       <c r="B58" s="27">
         <f>B57/B12/10000</f>
-        <v>0.2</v>
+        <v>0.12</v>
       </c>
       <c r="C58" s="27">
-        <f t="shared" ref="C58:F58" si="16">C57/C12/10000</f>
-        <v>0.15</v>
+        <f t="shared" ref="C58:F58" si="11">C57/C12/10000</f>
+        <v>0.12</v>
       </c>
       <c r="D58" s="27">
-        <f t="shared" si="16"/>
-        <v>0.1125</v>
+        <f t="shared" si="11"/>
+        <v>0.12</v>
       </c>
       <c r="E58" s="27">
-        <f t="shared" si="16"/>
-        <v>8.4375000000000006E-2</v>
+        <f t="shared" si="11"/>
+        <v>0.12</v>
       </c>
       <c r="F58" s="27">
-        <f t="shared" si="16"/>
-        <v>6.3281249999999997E-2</v>
+        <f t="shared" si="11"/>
+        <v>0.12</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -3041,23 +3052,23 @@
       </c>
       <c r="B60" s="12">
         <f>B59-B58</f>
-        <v>-8.0000000000000016E-2</v>
+        <v>0</v>
       </c>
       <c r="C60" s="12">
-        <f t="shared" ref="C60:F60" si="17">C59-C58</f>
-        <v>-0.03</v>
+        <f t="shared" ref="C60:F60" si="12">C59-C58</f>
+        <v>0</v>
       </c>
       <c r="D60" s="12">
-        <f t="shared" si="17"/>
-        <v>7.4999999999999928E-3</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
       <c r="E60" s="12">
-        <f t="shared" si="17"/>
-        <v>3.562499999999999E-2</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
       <c r="F60" s="12">
-        <f t="shared" si="17"/>
-        <v>5.6718749999999998E-2</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -3066,23 +3077,23 @@
       </c>
       <c r="B61" s="12">
         <f>B59/B58</f>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="C61" s="12">
-        <f t="shared" ref="C61:F61" si="18">C59/C58</f>
-        <v>0.8</v>
+        <f t="shared" ref="C61:F61" si="13">C59/C58</f>
+        <v>1</v>
       </c>
       <c r="D61" s="12">
-        <f t="shared" si="18"/>
-        <v>1.0666666666666667</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="E61" s="12">
-        <f t="shared" si="18"/>
-        <v>1.4222222222222221</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="F61" s="12">
-        <f t="shared" si="18"/>
-        <v>1.8962962962962964</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3093,15 +3104,1194 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="12" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="14">
+        <v>0</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14">
+        <v>2</v>
+      </c>
+      <c r="E9" s="14">
+        <v>3</v>
+      </c>
+      <c r="F9" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="13"/>
+      <c r="B10" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="17">
+        <f>$B$3*2^B9</f>
+        <v>6</v>
+      </c>
+      <c r="C12" s="17">
+        <f>$B$3*2^C9</f>
+        <v>12</v>
+      </c>
+      <c r="D12" s="17">
+        <f>$B$3*2^D9</f>
+        <v>24</v>
+      </c>
+      <c r="E12" s="17">
+        <f>$B$3*2^E9</f>
+        <v>48</v>
+      </c>
+      <c r="F12" s="17">
+        <f>$B$3*2^F9</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="D13" s="19">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E13" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="F13" s="19">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="18">
+        <f>B12*B13</f>
+        <v>3</v>
+      </c>
+      <c r="C14" s="18">
+        <f>C12*C13</f>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="D14" s="18">
+        <f>D12*D13</f>
+        <v>6.7200000000000006</v>
+      </c>
+      <c r="E14" s="18">
+        <f>E12*E13</f>
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="F14" s="18">
+        <f>F12*F13</f>
+        <v>14.399999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="18">
+        <v>25</v>
+      </c>
+      <c r="C15" s="18">
+        <v>25</v>
+      </c>
+      <c r="D15" s="18">
+        <v>25</v>
+      </c>
+      <c r="E15" s="18">
+        <v>25</v>
+      </c>
+      <c r="F15" s="18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="18">
+        <f>B15*B14</f>
+        <v>75</v>
+      </c>
+      <c r="C16" s="18">
+        <f>C15*C14</f>
+        <v>120.00000000000001</v>
+      </c>
+      <c r="D16" s="18">
+        <f>D15*D14</f>
+        <v>168.00000000000003</v>
+      </c>
+      <c r="E16" s="18">
+        <f>E15*E14</f>
+        <v>240.00000000000003</v>
+      </c>
+      <c r="F16" s="18">
+        <f>F15*F14</f>
+        <v>359.99999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="18">
+        <f>B16/B12</f>
+        <v>12.5</v>
+      </c>
+      <c r="C17" s="18">
+        <f>C16/C12</f>
+        <v>10.000000000000002</v>
+      </c>
+      <c r="D17" s="18">
+        <f>D16/D12</f>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="E17" s="18">
+        <f>E16/E12</f>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="F17" s="18">
+        <f>F16/F12</f>
+        <v>3.7499999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="18">
+        <v>9000</v>
+      </c>
+      <c r="C19" s="18">
+        <v>12000</v>
+      </c>
+      <c r="D19" s="18">
+        <v>14000</v>
+      </c>
+      <c r="E19" s="18">
+        <v>16000</v>
+      </c>
+      <c r="F19" s="18">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="20">
+        <f>B16*10000/B19</f>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="C20" s="20">
+        <f t="shared" ref="C20:F20" si="0">C16*10000/C19</f>
+        <v>100.00000000000001</v>
+      </c>
+      <c r="D20" s="20">
+        <f t="shared" si="0"/>
+        <v>120.00000000000001</v>
+      </c>
+      <c r="E20" s="20">
+        <f t="shared" si="0"/>
+        <v>150.00000000000003</v>
+      </c>
+      <c r="F20" s="20">
+        <f t="shared" si="0"/>
+        <v>199.99999999999997</v>
+      </c>
+      <c r="K20" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="L20" s="12">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="K21">
+        <v>54</v>
+      </c>
+      <c r="L21">
+        <v>36</v>
+      </c>
+      <c r="M21">
+        <f>K21+L21</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="19">
+        <v>0.15</v>
+      </c>
+      <c r="C22" s="19">
+        <v>0.13</v>
+      </c>
+      <c r="D22" s="19">
+        <v>0.12</v>
+      </c>
+      <c r="E22" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="F22" s="19">
+        <v>0.09</v>
+      </c>
+      <c r="K22">
+        <f>K20*K21</f>
+        <v>43.2</v>
+      </c>
+      <c r="L22">
+        <f>L20*L21</f>
+        <v>43.199999999999996</v>
+      </c>
+      <c r="M22">
+        <f>K22+L22</f>
+        <v>86.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="18">
+        <f>B12*B22*10000</f>
+        <v>9000</v>
+      </c>
+      <c r="C23" s="18">
+        <f t="shared" ref="C23:F23" si="1">C12*C22*10000</f>
+        <v>15600</v>
+      </c>
+      <c r="D23" s="18">
+        <f t="shared" si="1"/>
+        <v>28800</v>
+      </c>
+      <c r="E23" s="18">
+        <f t="shared" si="1"/>
+        <v>48000.000000000007</v>
+      </c>
+      <c r="F23" s="18">
+        <f t="shared" si="1"/>
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="18">
+        <v>9000</v>
+      </c>
+      <c r="C24" s="18">
+        <v>10000</v>
+      </c>
+      <c r="D24" s="18">
+        <v>12000</v>
+      </c>
+      <c r="E24" s="18">
+        <v>15000</v>
+      </c>
+      <c r="F24" s="18">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="18">
+        <f>(B23-B24)*10</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="18">
+        <f t="shared" ref="C25:F25" si="2">(C23-C24)*10</f>
+        <v>56000</v>
+      </c>
+      <c r="D25" s="18">
+        <f t="shared" si="2"/>
+        <v>168000</v>
+      </c>
+      <c r="E25" s="18">
+        <f t="shared" si="2"/>
+        <v>330000.00000000006</v>
+      </c>
+      <c r="F25" s="18">
+        <f t="shared" si="2"/>
+        <v>664000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="C27" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="E27" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="F27" s="19">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="18">
+        <f>B12*10000/$B$5</f>
+        <v>0.5</v>
+      </c>
+      <c r="C29" s="18">
+        <f>C12*10000/$B$5</f>
+        <v>1</v>
+      </c>
+      <c r="D29" s="18">
+        <f>D12*10000/$B$5</f>
+        <v>2</v>
+      </c>
+      <c r="E29" s="18">
+        <f>E12*10000/$B$5</f>
+        <v>4</v>
+      </c>
+      <c r="F29" s="18">
+        <f>F12*10000/$B$5</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="18">
+        <f>B29*$B$6/80</f>
+        <v>3.75</v>
+      </c>
+      <c r="C30" s="18">
+        <f t="shared" ref="C30:F30" si="3">C29*$B$6/80</f>
+        <v>7.5</v>
+      </c>
+      <c r="D30" s="18">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="E30" s="18">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="F30" s="18">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="18">
+        <f>B30*$B$7</f>
+        <v>93.75</v>
+      </c>
+      <c r="C31" s="18">
+        <f t="shared" ref="C31:F31" si="4">C30*$B$7</f>
+        <v>187.5</v>
+      </c>
+      <c r="D31" s="18">
+        <f t="shared" si="4"/>
+        <v>375</v>
+      </c>
+      <c r="E31" s="18">
+        <f t="shared" si="4"/>
+        <v>750</v>
+      </c>
+      <c r="F31" s="18">
+        <f t="shared" si="4"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="18">
+        <v>0</v>
+      </c>
+      <c r="B34" s="18">
+        <f t="shared" ref="B34:F42" si="5">B$31*$A34</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="18">
+        <v>50</v>
+      </c>
+      <c r="B35" s="23">
+        <f t="shared" si="5"/>
+        <v>4687.5</v>
+      </c>
+      <c r="C35" s="23">
+        <f t="shared" si="5"/>
+        <v>9375</v>
+      </c>
+      <c r="D35" s="23">
+        <f t="shared" si="5"/>
+        <v>18750</v>
+      </c>
+      <c r="E35" s="23">
+        <f t="shared" si="5"/>
+        <v>37500</v>
+      </c>
+      <c r="F35" s="23">
+        <f t="shared" si="5"/>
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="18">
+        <v>100</v>
+      </c>
+      <c r="B36" s="23">
+        <f t="shared" si="5"/>
+        <v>9375</v>
+      </c>
+      <c r="C36" s="23">
+        <f t="shared" si="5"/>
+        <v>18750</v>
+      </c>
+      <c r="D36" s="23">
+        <f t="shared" si="5"/>
+        <v>37500</v>
+      </c>
+      <c r="E36" s="23">
+        <f t="shared" si="5"/>
+        <v>75000</v>
+      </c>
+      <c r="F36" s="23">
+        <f t="shared" si="5"/>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="18">
+        <v>150</v>
+      </c>
+      <c r="B37" s="23">
+        <f t="shared" si="5"/>
+        <v>14062.5</v>
+      </c>
+      <c r="C37" s="23">
+        <f t="shared" si="5"/>
+        <v>28125</v>
+      </c>
+      <c r="D37" s="23">
+        <f t="shared" si="5"/>
+        <v>56250</v>
+      </c>
+      <c r="E37" s="23">
+        <f t="shared" si="5"/>
+        <v>112500</v>
+      </c>
+      <c r="F37" s="23">
+        <f t="shared" si="5"/>
+        <v>225000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="18">
+        <v>200</v>
+      </c>
+      <c r="B38" s="23">
+        <f t="shared" si="5"/>
+        <v>18750</v>
+      </c>
+      <c r="C38" s="23">
+        <f t="shared" si="5"/>
+        <v>37500</v>
+      </c>
+      <c r="D38" s="23">
+        <f t="shared" si="5"/>
+        <v>75000</v>
+      </c>
+      <c r="E38" s="23">
+        <f t="shared" si="5"/>
+        <v>150000</v>
+      </c>
+      <c r="F38" s="23">
+        <f t="shared" si="5"/>
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="18">
+        <v>250</v>
+      </c>
+      <c r="B39" s="23">
+        <f t="shared" si="5"/>
+        <v>23437.5</v>
+      </c>
+      <c r="C39" s="23">
+        <f t="shared" si="5"/>
+        <v>46875</v>
+      </c>
+      <c r="D39" s="23">
+        <f t="shared" si="5"/>
+        <v>93750</v>
+      </c>
+      <c r="E39" s="23">
+        <f t="shared" si="5"/>
+        <v>187500</v>
+      </c>
+      <c r="F39" s="23">
+        <f t="shared" si="5"/>
+        <v>375000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="18">
+        <v>300</v>
+      </c>
+      <c r="B40" s="23">
+        <f t="shared" si="5"/>
+        <v>28125</v>
+      </c>
+      <c r="C40" s="23">
+        <f t="shared" si="5"/>
+        <v>56250</v>
+      </c>
+      <c r="D40" s="23">
+        <f t="shared" si="5"/>
+        <v>112500</v>
+      </c>
+      <c r="E40" s="23">
+        <f t="shared" si="5"/>
+        <v>225000</v>
+      </c>
+      <c r="F40" s="23">
+        <f t="shared" si="5"/>
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="18">
+        <v>350</v>
+      </c>
+      <c r="B41" s="23">
+        <f t="shared" si="5"/>
+        <v>32812.5</v>
+      </c>
+      <c r="C41" s="23">
+        <f t="shared" si="5"/>
+        <v>65625</v>
+      </c>
+      <c r="D41" s="23">
+        <f t="shared" si="5"/>
+        <v>131250</v>
+      </c>
+      <c r="E41" s="23">
+        <f t="shared" si="5"/>
+        <v>262500</v>
+      </c>
+      <c r="F41" s="23">
+        <f t="shared" si="5"/>
+        <v>525000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="18">
+        <v>400</v>
+      </c>
+      <c r="B42" s="23">
+        <f t="shared" si="5"/>
+        <v>37500</v>
+      </c>
+      <c r="C42" s="23">
+        <f t="shared" si="5"/>
+        <v>75000</v>
+      </c>
+      <c r="D42" s="23">
+        <f t="shared" si="5"/>
+        <v>150000</v>
+      </c>
+      <c r="E42" s="23">
+        <f t="shared" si="5"/>
+        <v>300000</v>
+      </c>
+      <c r="F42" s="23">
+        <f t="shared" si="5"/>
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="18">
+        <v>0</v>
+      </c>
+      <c r="B44" s="23">
+        <f>B42</f>
+        <v>37500</v>
+      </c>
+      <c r="C44" s="25">
+        <f t="shared" ref="C44:F44" si="6">C42</f>
+        <v>75000</v>
+      </c>
+      <c r="D44" s="25">
+        <f t="shared" si="6"/>
+        <v>150000</v>
+      </c>
+      <c r="E44" s="25">
+        <f t="shared" si="6"/>
+        <v>300000</v>
+      </c>
+      <c r="F44" s="23">
+        <f t="shared" si="6"/>
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="18">
+        <v>50</v>
+      </c>
+      <c r="B45" s="23">
+        <f>B$44-B35</f>
+        <v>32812.5</v>
+      </c>
+      <c r="C45" s="25">
+        <f t="shared" ref="C45:F45" si="7">C$44-C35</f>
+        <v>65625</v>
+      </c>
+      <c r="D45" s="25">
+        <f t="shared" si="7"/>
+        <v>131250</v>
+      </c>
+      <c r="E45" s="25">
+        <f t="shared" si="7"/>
+        <v>262500</v>
+      </c>
+      <c r="F45" s="23">
+        <f t="shared" si="7"/>
+        <v>525000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="18">
+        <v>100</v>
+      </c>
+      <c r="B46" s="23">
+        <f t="shared" ref="B46:F46" si="8">B$44-B36</f>
+        <v>28125</v>
+      </c>
+      <c r="C46" s="25">
+        <f t="shared" si="8"/>
+        <v>56250</v>
+      </c>
+      <c r="D46" s="25">
+        <f t="shared" si="8"/>
+        <v>112500</v>
+      </c>
+      <c r="E46" s="25">
+        <f t="shared" si="8"/>
+        <v>225000</v>
+      </c>
+      <c r="F46" s="23">
+        <f t="shared" si="8"/>
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="18">
+        <v>150</v>
+      </c>
+      <c r="B47" s="23">
+        <f t="shared" ref="B47:F47" si="9">B$44-B37</f>
+        <v>23437.5</v>
+      </c>
+      <c r="C47" s="23">
+        <f t="shared" si="9"/>
+        <v>46875</v>
+      </c>
+      <c r="D47" s="23">
+        <f t="shared" si="9"/>
+        <v>93750</v>
+      </c>
+      <c r="E47" s="23">
+        <f t="shared" si="9"/>
+        <v>187500</v>
+      </c>
+      <c r="F47" s="23">
+        <f t="shared" si="9"/>
+        <v>375000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="18">
+        <v>200</v>
+      </c>
+      <c r="B48" s="23">
+        <f t="shared" ref="B48:F48" si="10">B$44-B38</f>
+        <v>18750</v>
+      </c>
+      <c r="C48" s="23">
+        <f t="shared" si="10"/>
+        <v>37500</v>
+      </c>
+      <c r="D48" s="23">
+        <f t="shared" si="10"/>
+        <v>75000</v>
+      </c>
+      <c r="E48" s="23">
+        <f t="shared" si="10"/>
+        <v>150000</v>
+      </c>
+      <c r="F48" s="23">
+        <f t="shared" si="10"/>
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="18">
+        <v>250</v>
+      </c>
+      <c r="B49" s="23">
+        <f t="shared" ref="B49:F49" si="11">B$44-B39</f>
+        <v>14062.5</v>
+      </c>
+      <c r="C49" s="23">
+        <f t="shared" si="11"/>
+        <v>28125</v>
+      </c>
+      <c r="D49" s="23">
+        <f t="shared" si="11"/>
+        <v>56250</v>
+      </c>
+      <c r="E49" s="23">
+        <f t="shared" si="11"/>
+        <v>112500</v>
+      </c>
+      <c r="F49" s="23">
+        <f t="shared" si="11"/>
+        <v>225000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="18">
+        <v>300</v>
+      </c>
+      <c r="B50" s="23">
+        <f t="shared" ref="B50:F50" si="12">B$44-B40</f>
+        <v>9375</v>
+      </c>
+      <c r="C50" s="23">
+        <f t="shared" si="12"/>
+        <v>18750</v>
+      </c>
+      <c r="D50" s="23">
+        <f t="shared" si="12"/>
+        <v>37500</v>
+      </c>
+      <c r="E50" s="23">
+        <f t="shared" si="12"/>
+        <v>75000</v>
+      </c>
+      <c r="F50" s="23">
+        <f t="shared" si="12"/>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="18">
+        <v>350</v>
+      </c>
+      <c r="B51" s="23">
+        <f t="shared" ref="B51:F51" si="13">B$44-B41</f>
+        <v>4687.5</v>
+      </c>
+      <c r="C51" s="23">
+        <f t="shared" si="13"/>
+        <v>9375</v>
+      </c>
+      <c r="D51" s="23">
+        <f t="shared" si="13"/>
+        <v>18750</v>
+      </c>
+      <c r="E51" s="23">
+        <f t="shared" si="13"/>
+        <v>37500</v>
+      </c>
+      <c r="F51" s="23">
+        <f t="shared" si="13"/>
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="18">
+        <v>400</v>
+      </c>
+      <c r="B52" s="23">
+        <f t="shared" ref="B52:F52" si="14">B$44-B42</f>
+        <v>0</v>
+      </c>
+      <c r="C52" s="23">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="D52" s="23">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="23">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="23">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="18"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="H55" t="s">
+        <v>54</v>
+      </c>
+      <c r="I55" s="28">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="H56" t="s">
+        <v>53</v>
+      </c>
+      <c r="I56" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" s="26">
+        <f>$I$55*$I$56^B9</f>
+        <v>12000</v>
+      </c>
+      <c r="C57" s="26">
+        <f t="shared" ref="C57:F57" si="15">$I$55*$I$56^C9</f>
+        <v>18000</v>
+      </c>
+      <c r="D57" s="26">
+        <f t="shared" si="15"/>
+        <v>27000</v>
+      </c>
+      <c r="E57" s="26">
+        <f t="shared" si="15"/>
+        <v>40500</v>
+      </c>
+      <c r="F57" s="26">
+        <f t="shared" si="15"/>
+        <v>60750</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" s="27">
+        <f>B57/B12/10000</f>
+        <v>0.2</v>
+      </c>
+      <c r="C58" s="27">
+        <f t="shared" ref="C58:F58" si="16">C57/C12/10000</f>
+        <v>0.15</v>
+      </c>
+      <c r="D58" s="27">
+        <f t="shared" si="16"/>
+        <v>0.1125</v>
+      </c>
+      <c r="E58" s="27">
+        <f t="shared" si="16"/>
+        <v>8.4375000000000006E-2</v>
+      </c>
+      <c r="F58" s="27">
+        <f t="shared" si="16"/>
+        <v>6.3281249999999997E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="C59" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="D59" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="E59" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="F59" s="12">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="12">
+        <f>B59-B58</f>
+        <v>-8.0000000000000016E-2</v>
+      </c>
+      <c r="C60" s="12">
+        <f t="shared" ref="C60:F60" si="17">C59-C58</f>
+        <v>-0.03</v>
+      </c>
+      <c r="D60" s="12">
+        <f t="shared" si="17"/>
+        <v>7.4999999999999928E-3</v>
+      </c>
+      <c r="E60" s="12">
+        <f t="shared" si="17"/>
+        <v>3.562499999999999E-2</v>
+      </c>
+      <c r="F60" s="12">
+        <f t="shared" si="17"/>
+        <v>5.6718749999999998E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" s="12">
+        <f>B59/B58</f>
+        <v>0.6</v>
+      </c>
+      <c r="C61" s="12">
+        <f t="shared" ref="C61:F61" si="18">C59/C58</f>
+        <v>0.8</v>
+      </c>
+      <c r="D61" s="12">
+        <f t="shared" si="18"/>
+        <v>1.0666666666666667</v>
+      </c>
+      <c r="E61" s="12">
+        <f t="shared" si="18"/>
+        <v>1.4222222222222221</v>
+      </c>
+      <c r="F61" s="12">
+        <f t="shared" si="18"/>
+        <v>1.8962962962962964</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.453125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:11">
@@ -3172,15 +4362,15 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="5"/>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30" t="s">
+      <c r="C10" s="31"/>
+      <c r="D10" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -3420,15 +4610,15 @@
       </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31" t="s">
+      <c r="C22" s="32"/>
+      <c r="D22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
     </row>
     <row r="23" spans="1:11">
       <c r="B23" s="4">
@@ -3518,7 +4708,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:K24"/>
   <sheetViews>
@@ -3526,9 +4716,9 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.453125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:11">
@@ -3599,15 +4789,15 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="5"/>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="29" t="s">
+      <c r="C10" s="31"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="30"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -3826,15 +5016,15 @@
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="29" t="s">
+      <c r="C21" s="31"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="30"/>
+      <c r="F21" s="31"/>
     </row>
     <row r="22" spans="1:11">
       <c r="B22" s="4">
@@ -3919,7 +5109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:M39"/>
   <sheetViews>
@@ -3927,9 +5117,9 @@
       <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.453125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:11">
@@ -4013,15 +5203,15 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="5"/>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30" t="s">
+      <c r="C10" s="31"/>
+      <c r="D10" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -4271,15 +5461,15 @@
       </c>
     </row>
     <row r="22" spans="1:13">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31" t="s">
+      <c r="C22" s="32"/>
+      <c r="D22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
     </row>
     <row r="23" spans="1:13">
       <c r="B23" s="4">

</xml_diff>